<commit_message>
Incorporated latest features: new prompt type 'public_question' and 'private_question' to either allow participants from the same round to either see or not see other responses, included permutation information during experiment printout, included temperature definition, allow response_options to include support for strings, included new column for formatting responses into JSON for easy parsing
</commit_message>
<xml_diff>
--- a/demos/public_good_experiment_prompt_template_sample.xlsx
+++ b/demos/public_good_experiment_prompt_template_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondlow/Documents/talking-to-machines/talking-to-machines/demos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DC51E7-497A-964F-9030-442D70F22811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008903A3-520D-644A-BDE8-41CC4530EBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1580" yWindow="-22560" windowWidth="36220" windowHeight="21460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8680" yWindow="760" windowWidth="25880" windowHeight="20240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="experimental_setting" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="129">
   <si>
     <t>experimental_setting</t>
   </si>
@@ -162,6 +162,297 @@
   </si>
   <si>
     <t>context</t>
+  </si>
+  <si>
+    <t>experiment_context</t>
+  </si>
+  <si>
+    <t>Please answer the following questions to ensure you understand the rules. If you contribute 5 tokens to the public account, how many total tokens will be in the public account before it is shared?</t>
+  </si>
+  <si>
+    <t>comprehension_qn_1</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>[10, 15, 20, 25]</t>
+  </si>
+  <si>
+    <t>Please answer the following questions to ensure you understand the rules. How are tokens from the public account distributed to group members?</t>
+  </si>
+  <si>
+    <t>comprehension_qn_2</t>
+  </si>
+  <si>
+    <t>["Equally among all members", "Based on individual contributions", "Randomly assigned", "Not distributed at all"]</t>
+  </si>
+  <si>
+    <t>Please answer the following questions to ensure you understand the rules. If you keep all your tokens in your private account, what happens to the tokens in the public account?</t>
+  </si>
+  <si>
+    <t>comprehension_qn_3</t>
+  </si>
+  <si>
+    <t>["You receive nothing from the public account", "The total tokens in the public account decrease", "Other group members’ earnings increase", "None of the above"]</t>
+  </si>
+  <si>
+    <t>How many tokens do you want to contribute to the public account? (Enter a number between 0 and 10)</t>
+  </si>
+  <si>
+    <t>round_decision_1</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>round_decision_2</t>
+  </si>
+  <si>
+    <t>round_decision_3</t>
+  </si>
+  <si>
+    <t>round_decision_4</t>
+  </si>
+  <si>
+    <t>round_decision_5</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>college</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>knowledge_counter</t>
+  </si>
+  <si>
+    <t>extraversion</t>
+  </si>
+  <si>
+    <t>agreeable</t>
+  </si>
+  <si>
+    <t>consecientious</t>
+  </si>
+  <si>
+    <t>emotionally_stable</t>
+  </si>
+  <si>
+    <t>open_new_experiences</t>
+  </si>
+  <si>
+    <t>political_interest</t>
+  </si>
+  <si>
+    <t>strong_partisan</t>
+  </si>
+  <si>
+    <t>percent_other_party_exposure</t>
+  </si>
+  <si>
+    <t>democrat</t>
+  </si>
+  <si>
+    <t>sevenpoint_ideology</t>
+  </si>
+  <si>
+    <t>regionMidwest</t>
+  </si>
+  <si>
+    <t>regionSouth</t>
+  </si>
+  <si>
+    <t>regionWest</t>
+  </si>
+  <si>
+    <t>republican</t>
+  </si>
+  <si>
+    <t>What is your gender? 1 refers to Male and 2 refers to Female</t>
+  </si>
+  <si>
+    <t>What is your age?</t>
+  </si>
+  <si>
+    <t>Do you have a college education?</t>
+  </si>
+  <si>
+    <t>Are you white?</t>
+  </si>
+  <si>
+    <t>On a scale from 0 to 3, where 0 means "Not at All Knowledgeable" and 3 means "Very Knowledgeable," please rate the following statement: I consider myself knowledgeable about political issues and events.</t>
+  </si>
+  <si>
+    <t>On a scale from 1 to 7, where 1 means "Disagree Strongly" and 7 means "Agree Strongly", how well do the following statement describe your personality: I see myself as someone who is extraverted, enthusiastic, unreserved, and loud.</t>
+  </si>
+  <si>
+    <t>On a scale from 1 to 7, where 1 means "Disagree Strongly" and 7 means "Agree Strongly", how well do the following statement describe your personality: I see myself as someone who is uncritical, peaceful, sympathetic, and warm.</t>
+  </si>
+  <si>
+    <t>On a scale from 1 to 7, where 1 means "Disagree Strongly" and 7 means "Agree Strongly", how well do the following statement describe your personality: I see myself as someone who dependable, self-disciplined, organised, and careful.</t>
+  </si>
+  <si>
+    <t>On a scale from 1 to 7, where 1 means "Disagree Strongly" and 7 means "Agree Strongly", how well do the following statement describe your personality: I see myself as someone who is calm, not easily upset, calm, emotionally stable.</t>
+  </si>
+  <si>
+    <t>On a scale from 1 to 7, where 1 means "Disagree Strongly" and 7 means "Agree Strongly", how well do the following statement describe your personality: I see myself as someone who is open to new experiences, complex, unconventional, and creative.</t>
+  </si>
+  <si>
+    <t>On a scale from 1 to 4, where 1 means "Not at All Interested" and 4 means "Very Interested," please rate your level of interest in politics.</t>
+  </si>
+  <si>
+    <t>Do you strongly align with your current political party and actively support its policies and candidates?</t>
+  </si>
+  <si>
+    <t>On a scale from 0 to 100, where 0 means "No Exposure" and 100 means "Extensive Exposure," please indicate the percentage of your political information and interactions that come from sources affiliated with parties other than your own.</t>
+  </si>
+  <si>
+    <t>Are you a democrat?</t>
+  </si>
+  <si>
+    <t>On a scale from 1 to 7, where 1 means "Very Liberal," 4 means "Moderate," and 7 means "Very Conservative," please rate your political ideology.</t>
+  </si>
+  <si>
+    <t>Do you live in the midwest region of the United States?</t>
+  </si>
+  <si>
+    <t>Do you live in the south region of the United States?</t>
+  </si>
+  <si>
+    <t>Do you live in the west region of the United States?</t>
+  </si>
+  <si>
+    <t>Are you a republican?</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>participant_label</t>
+  </si>
+  <si>
+    <t>random_seed</t>
+  </si>
+  <si>
+    <t>session_column</t>
+  </si>
+  <si>
+    <t>role_column</t>
+  </si>
+  <si>
+    <t>treatment_column</t>
+  </si>
+  <si>
+    <t>Summarizer</t>
+  </si>
+  <si>
+    <t>(0,10)</t>
+  </si>
+  <si>
+    <t>Please answer the following questions to ensure you understand the rules. If you contribute 5 tokens to the public account, how many total tokens will be in the public account before it is shared? {response_options}</t>
+  </si>
+  <si>
+    <t>Please answer the following questions to ensure you understand the rules. How are tokens from the public account distributed to group members? {response_options}</t>
+  </si>
+  <si>
+    <t>Please answer the following questions to ensure you understand the rules. If you keep all your tokens in your private account, what happens to the tokens in the public account? {response_options}</t>
+  </si>
+  <si>
+    <t>public_good_experiment_sample</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>format_response</t>
+  </si>
+  <si>
+    <t>Enter a number between 0 and 10</t>
+  </si>
+  <si>
+    <t>{"Participant 1": "How many tokens do you want to contribute to the public account? {response_options}", "Participant 2": "How many tokens do you want to contribute to the public account? {response_options}", "Participant 3": "How many tokens do you want to contribute to the public account? {response_options}", "Participant 4": "How many tokens do you want to contribute to the public account? {response_options}", "Summarizer": "Calculate the following information for each participant in the following format:\n- The total tokens contributed to the public account by all participants:\n- The participant's earnings from the public account:\n- The participant's private tokens kept from the round:\n- The participant's total earnings so far:"}</t>
+  </si>
+  <si>
+    <t>[0,1,2,3,4,5,6,7,8,9,10]</t>
+  </si>
+  <si>
+    <t>{"Participant 1": "Enter a number between 0 and 10", "Participant 2": "Enter a number between 0 and 10", "Participant 3": (0,10), "Participant 4": [0,1,2,3,4,5,6,7,8,9,10]}</t>
+  </si>
+  <si>
+    <t>public_question</t>
+  </si>
+  <si>
+    <t>private_question</t>
+  </si>
+  <si>
+    <t>{"Participant 4": "How many tokens do you want to contribute to the public account? {response_options}", "Participant 3": "How many tokens do you want to contribute to the public account? {response_options}", "Participant 2": "How many tokens do you want to contribute to the public account? {response_options}", "Participant 1": "How many tokens do you want to contribute to the public account? {response_options}", "Summarizer": "Calculate the following information for each participant in the following format:\n- The total tokens contributed to the public account by all participants:\n- The participant's earnings from the public account:\n- The participant's private tokens kept from the round:\n- The participant's total earnings so far:"}</t>
+  </si>
+  <si>
+    <t>["participant", "subject"]</t>
+  </si>
+  <si>
+    <t>Assume the role of a summariser in a public good experiment involving 4 {{participant_label}}s. Each {{participant_label}} will start with an initial endowment of 10 tokens. During each round of the experiment, each {{participant_label}} is asked to decide how many tokens to contribute to a public account and how many to keep in their private account. The tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in the {{participant_label}}s' private account will not be shared and remain private. 
+Example:
+A {{participant_label}} have 10 tokens. If that {{participant_label}} contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 / 4). The {{participant_label}} will keep the remaining 6 tokens in their private account. Contributions to the public account benefit everyone, including the {{participant_label}}. What they keep in their private account benefits only themselves. The total earnings for each round equal to private tokens kept + public tokens earned.
+At the end of each round, you are responsible for calculating the following information for each {{participant_label}}:
+- The total tokens contributed to the public account by all {{participant_label}}s.
+- The {{participant_label}}'s earnings from the public account.
+- The {{participant_label}}'s private tokens kept from the round.
+- The {{participant_label}}'s total earnings so far.</t>
+  </si>
+  <si>
+    <t>Assume the role of a {{participant_label}} (Participant 1) in a public good experiment involving 3 other {{participant_label}}s. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
+Example: 
+You have 10 tokens. If you contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 / 4). You will keep the remaining 6 tokens in your private account. Contributions to the public account benefit everyone, including you. What you keep in your private account benefits only you. Your total earnings for each round equal to private tokens kept + public tokens earned.
+At the end of each round, you will see:
+- The total tokens contributed to the public account by all {{participant_label}}s.
+- Your earnings from the public account.
+- Your private tokens kept from the round.
+- Your total earnings so far.
+Answer any question that is posed to you in as much detail as possible and in the format required. Please provide a consistent and coherent response using all the demographic information provided about you. It is crucial for you to accurately replicate the response of a human subject that has the demographic profile you are provided. The human subject response will vary depending on their demographic profile. If you are unsure of an answer, provide a plausible response that is based on all of the information available to you. Do not include your name in your response.</t>
+  </si>
+  <si>
+    <t>Assume the role of a {{participant_label}} (Participant 2) in a public good experiment involving 3 other {{participant_label}}s. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
+Example: 
+You have 10 tokens. If you contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 / 4). You will keep the remaining 6 tokens in your private account. Contributions to the public account benefit everyone, including you. What you keep in your private account benefits only you. Your total earnings for each round equal to private tokens kept + public tokens earned.
+At the end of each round, you will see:
+- The total tokens contributed to the public account by all {{participant_label}}s.
+- Your earnings from the public account.
+- Your private tokens kept from the round.
+- Your total earnings so far.
+Answer any question that is posed to you in as much detail as possible and in the format required. Please provide a consistent and coherent response using all the demographic information provided about you. It is crucial for you to accurately replicate the response of a human subject that has the demographic profile you are provided. The human subject response will vary depending on their demographic profile. If you are unsure of an answer, provide a plausible response that is based on all of the information available to you. Do not include your name in your response.</t>
+  </si>
+  <si>
+    <t>Assume the role of a {{participant_label}} (Participant 3) in a public good experiment involving 3 other {{participant_label}}s. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
+Example: 
+You have 10 tokens. If you contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 / 4). You will keep the remaining 6 tokens in your private account. Contributions to the public account benefit everyone, including you. What you keep in your private account benefits only you. Your total earnings for each round equal to private tokens kept + public tokens earned.
+At the end of each round, you will see:
+- The total tokens contributed to the public account by all {{participant_label}}s.
+- Your earnings from the public account.
+- Your private tokens kept from the round.
+- Your total earnings so far.
+Answer any question that is posed to you in as much detail as possible and in the format required. Please provide a consistent and coherent response using all the demographic information provided about you. It is crucial for you to accurately replicate the response of a human subject that has the demographic profile you are provided. The human subject response will vary depending on their demographic profile. If you are unsure of an answer, provide a plausible response that is based on all of the information available to you. Do not include your name in your response.</t>
+  </si>
+  <si>
+    <t>Assume the role of a {{participant_label}} (Participant 4) in a public good experiment involving 3 other {{participant_label}}s. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
+Example: 
+You have 10 tokens. If you contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 / 4). You will keep the remaining 6 tokens in your private account. Contributions to the public account benefit everyone, including you. What you keep in your private account benefits only you. Your total earnings for each round equal to private tokens kept + public tokens earned.
+At the end of each round, you will see:
+- The total tokens contributed to the public account by all {{participant_label}}s.
+- Your earnings from the public account.
+- Your private tokens kept from the round.
+- Your total earnings so far.
+Answer any question that is posed to you in as much detail as possible and in the format required. Please provide a consistent and coherent response using all the demographic information provided about you. It is crucial for you to accurately replicate the response of a human subject that has the demographic profile you are provided. The human subject response will vary depending on their demographic profile. If you are unsure of an answer, provide a plausible response that is based on all of the information available to you. Do not include your name in your response.</t>
   </si>
   <si>
     <t xml:space="preserve">General Overview
@@ -174,7 +465,7 @@
 You have 10 tokens.
 If you contribute 4 tokens to the public account:
 These 4 tokens are doubled to 8 and shared equally among the group.
-Each group member receives 2 tokens (8 ÷ 4).
+Each group member receives 2 tokens (8 / 4).
 You keep the remaining 6 tokens in your private account.
 Contributions to the public account benefit everyone, including you.
 What you keep in your private account benefits only you.
@@ -188,206 +479,8 @@
 </t>
   </si>
   <si>
-    <t>experiment_context</t>
-  </si>
-  <si>
-    <t>question</t>
-  </si>
-  <si>
-    <t>Please answer the following questions to ensure you understand the rules. If you contribute 5 tokens to the public account, how many total tokens will be in the public account before it is shared?</t>
-  </si>
-  <si>
-    <t>comprehension_qn_1</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>[10, 15, 20, 25]</t>
-  </si>
-  <si>
-    <t>Please answer the following questions to ensure you understand the rules. How are tokens from the public account distributed to group members?</t>
-  </si>
-  <si>
-    <t>comprehension_qn_2</t>
-  </si>
-  <si>
-    <t>["Equally among all members", "Based on individual contributions", "Randomly assigned", "Not distributed at all"]</t>
-  </si>
-  <si>
-    <t>Please answer the following questions to ensure you understand the rules. If you keep all your tokens in your private account, what happens to the tokens in the public account?</t>
-  </si>
-  <si>
-    <t>comprehension_qn_3</t>
-  </si>
-  <si>
-    <t>["You receive nothing from the public account", "The total tokens in the public account decrease", "Other group members’ earnings increase", "None of the above"]</t>
-  </si>
-  <si>
-    <t>How many tokens do you want to contribute to the public account? (Enter a number between 0 and 10)</t>
-  </si>
-  <si>
-    <t>round_decision_1</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>round_decision_2</t>
-  </si>
-  <si>
-    <t>round_decision_3</t>
-  </si>
-  <si>
-    <t>round_decision_4</t>
-  </si>
-  <si>
-    <t>round_decision_5</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>college</t>
-  </si>
-  <si>
-    <t>white</t>
-  </si>
-  <si>
-    <t>knowledge_counter</t>
-  </si>
-  <si>
-    <t>extraversion</t>
-  </si>
-  <si>
-    <t>agreeable</t>
-  </si>
-  <si>
-    <t>consecientious</t>
-  </si>
-  <si>
-    <t>emotionally_stable</t>
-  </si>
-  <si>
-    <t>open_new_experiences</t>
-  </si>
-  <si>
-    <t>political_interest</t>
-  </si>
-  <si>
-    <t>strong_partisan</t>
-  </si>
-  <si>
-    <t>percent_other_party_exposure</t>
-  </si>
-  <si>
-    <t>democrat</t>
-  </si>
-  <si>
-    <t>sevenpoint_ideology</t>
-  </si>
-  <si>
-    <t>regionMidwest</t>
-  </si>
-  <si>
-    <t>regionSouth</t>
-  </si>
-  <si>
-    <t>regionWest</t>
-  </si>
-  <si>
-    <t>republican</t>
-  </si>
-  <si>
-    <t>What is your gender? 1 refers to Male and 2 refers to Female</t>
-  </si>
-  <si>
-    <t>What is your age?</t>
-  </si>
-  <si>
-    <t>Do you have a college education?</t>
-  </si>
-  <si>
-    <t>Are you white?</t>
-  </si>
-  <si>
-    <t>On a scale from 0 to 3, where 0 means "Not at All Knowledgeable" and 3 means "Very Knowledgeable," please rate the following statement: I consider myself knowledgeable about political issues and events.</t>
-  </si>
-  <si>
-    <t>On a scale from 1 to 7, where 1 means "Disagree Strongly" and 7 means "Agree Strongly", how well do the following statement describe your personality: I see myself as someone who is extraverted, enthusiastic, unreserved, and loud.</t>
-  </si>
-  <si>
-    <t>On a scale from 1 to 7, where 1 means "Disagree Strongly" and 7 means "Agree Strongly", how well do the following statement describe your personality: I see myself as someone who is uncritical, peaceful, sympathetic, and warm.</t>
-  </si>
-  <si>
-    <t>On a scale from 1 to 7, where 1 means "Disagree Strongly" and 7 means "Agree Strongly", how well do the following statement describe your personality: I see myself as someone who dependable, self-disciplined, organised, and careful.</t>
-  </si>
-  <si>
-    <t>On a scale from 1 to 7, where 1 means "Disagree Strongly" and 7 means "Agree Strongly", how well do the following statement describe your personality: I see myself as someone who is calm, not easily upset, calm, emotionally stable.</t>
-  </si>
-  <si>
-    <t>On a scale from 1 to 7, where 1 means "Disagree Strongly" and 7 means "Agree Strongly", how well do the following statement describe your personality: I see myself as someone who is open to new experiences, complex, unconventional, and creative.</t>
-  </si>
-  <si>
-    <t>On a scale from 1 to 4, where 1 means "Not at All Interested" and 4 means "Very Interested," please rate your level of interest in politics.</t>
-  </si>
-  <si>
-    <t>Do you strongly align with your current political party and actively support its policies and candidates?</t>
-  </si>
-  <si>
-    <t>On a scale from 0 to 100, where 0 means "No Exposure" and 100 means "Extensive Exposure," please indicate the percentage of your political information and interactions that come from sources affiliated with parties other than your own.</t>
-  </si>
-  <si>
-    <t>Are you a democrat?</t>
-  </si>
-  <si>
-    <t>On a scale from 1 to 7, where 1 means "Very Liberal," 4 means "Moderate," and 7 means "Very Conservative," please rate your political ideology.</t>
-  </si>
-  <si>
-    <t>Do you live in the midwest region of the United States?</t>
-  </si>
-  <si>
-    <t>Do you live in the south region of the United States?</t>
-  </si>
-  <si>
-    <t>Do you live in the west region of the United States?</t>
-  </si>
-  <si>
-    <t>Are you a republican?</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>participant_label</t>
-  </si>
-  <si>
-    <t>["participants", "subjects"]</t>
-  </si>
-  <si>
-    <t>random_seed</t>
-  </si>
-  <si>
-    <t>session_column</t>
-  </si>
-  <si>
-    <t>role_column</t>
-  </si>
-  <si>
-    <t>treatment_column</t>
-  </si>
-  <si>
-    <t>Summarizer</t>
-  </si>
-  <si>
     <t xml:space="preserve">General Overview
-Welcome to the public good experiment. You will be part of a group of 4 {{participant_label}}, and you will interact with the same group throughout the experiment. The experiment consists of 5 rounds, and your decisions will affect both your earnings and the earnings of others in your group. All decisions are anonymous, and you will not know the identity of other {{participant_label}}.
+Welcome to the public good experiment. You will be part of a group of 4 {{participant_label}}s, and you will interact with the same group throughout the experiment. The experiment consists of 5 rounds, and your decisions will affect both your earnings and the earnings of others in your group. All decisions are anonymous, and you will not know the identity of other {{participant_label}}s.
 1. Instructions
 Your group will start with an initial endowment of 10 tokens.
 You must decide how many tokens to contribute to a public account and how many to keep in your private account.
@@ -396,7 +489,7 @@
 You have 10 tokens.
 If you contribute 4 tokens to the public account:
 These 4 tokens are doubled to 8 and shared equally among the group.
-Each group member receives 2 tokens (8 ÷ 4).
+Each group member receives 2 tokens (8 / 4).
 You keep the remaining 6 tokens in your private account.
 Contributions to the public account benefit everyone, including you.
 What you keep in your private account benefits only you.
@@ -408,81 +501,6 @@
 Your private tokens kept from the round.
 Your total earnings so far.
 </t>
-  </si>
-  <si>
-    <t>(0,10)</t>
-  </si>
-  <si>
-    <t>{"Participant 1": (0,10), "Participant 2": (0,10), "Participant 3": (0,10), "Participant 4": (0,10)}</t>
-  </si>
-  <si>
-    <t>Assume the role of a summariser in a public good experiment involving 4 {{participant_label}}. Each {{participant_label}} will start with an initial endowment of 10 tokens. During each round of the experiment, each {{participant_label}} is asked to decide how many tokens to contribute to a public account and how many to keep in their private account. The tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in the {{participant_label}}s' private account will not be shared and remain private. 
-Example:
-A {{participant_label}} have 10 tokens. If that {{participant_label}} contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 ÷ 4). The {{participant_label}} will keep the remaining 6 tokens in their private account. Contributions to the public account benefit everyone, including the {{participant_label}}. What they keep in their private account benefits only themselves. The total earnings for each round equal to private tokens kept + public tokens earned.
-At the end of each round, you are responsible for calculating the following information for each {{participant_label}}:
-- The total tokens contributed to the public account by all {{participant_label}}s.
-- The {{participant_label}}'s earnings from the public account.
-- The {{participant_label}}'s private tokens kept from the round.
-- The {{participant_label}}'s total earnings so far.</t>
-  </si>
-  <si>
-    <t>Assume the role of a {{participant_label}} (Participant 1) in a public good experiment involving 3 other {{participant_label}}s. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
-Example: 
-You have 10 tokens. If you contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 ÷ 4). You will keep the remaining 6 tokens in your private account. Contributions to the public account benefit everyone, including you. What you keep in your private account benefits only you. Your total earnings for each round equal to private tokens kept + public tokens earned.
-At the end of each round, you will see:
-- The total tokens contributed to the public account by all {{participant_label}}s.
-- Your earnings from the public account.
-- Your private tokens kept from the round.
-- Your total earnings so far.
-Answer any question that is posed to you in as much detail as possible and in the format required. Please provide a consistent and coherent response using all the demographic information provided about you. It is crucial for you to accurately replicate the response of a human subject that has the demographic profile you are provided. The human subject response will vary depending on their demographic profile. If you are unsure of an answer, provide a plausible response that is based on all of the information available to you. Do not include your name in your response.</t>
-  </si>
-  <si>
-    <t>Assume the role of a {{participant_label}} (Participant 2) in a public good experiment involving 3 other {{participant_label}}s. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
-Example: 
-You have 10 tokens. If you contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 ÷ 4). You will keep the remaining 6 tokens in your private account. Contributions to the public account benefit everyone, including you. What you keep in your private account benefits only you. Your total earnings for each round equal to private tokens kept + public tokens earned.
-At the end of each round, you will see:
-- The total tokens contributed to the public account by all {{participant_label}}s.
-- Your earnings from the public account.
-- Your private tokens kept from the round.
-- Your total earnings so far.
-Answer any question that is posed to you in as much detail as possible and in the format required. Please provide a consistent and coherent response using all the demographic information provided about you. It is crucial for you to accurately replicate the response of a human subject that has the demographic profile you are provided. The human subject response will vary depending on their demographic profile. If you are unsure of an answer, provide a plausible response that is based on all of the information available to you. Do not include your name in your response.</t>
-  </si>
-  <si>
-    <t>Assume the role of a {{participant_label}} (Participant 3) in a public good experiment involving 3 other {{participant_label}}s. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
-Example: 
-You have 10 tokens. If you contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 ÷ 4). You will keep the remaining 6 tokens in your private account. Contributions to the public account benefit everyone, including you. What you keep in your private account benefits only you. Your total earnings for each round equal to private tokens kept + public tokens earned.
-At the end of each round, you will see:
-- The total tokens contributed to the public account by all {{participant_label}}s.
-- Your earnings from the public account.
-- Your private tokens kept from the round.
-- Your total earnings so far.
-Answer any question that is posed to you in as much detail as possible and in the format required. Please provide a consistent and coherent response using all the demographic information provided about you. It is crucial for you to accurately replicate the response of a human subject that has the demographic profile you are provided. The human subject response will vary depending on their demographic profile. If you are unsure of an answer, provide a plausible response that is based on all of the information available to you. Do not include your name in your response.</t>
-  </si>
-  <si>
-    <t>Assume the role of a {{participant_label}} (Participant 4) in a public good experiment involving 3 other {{participant_label}}s. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
-Example: 
-You have 10 tokens. If you contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 ÷ 4). You will keep the remaining 6 tokens in your private account. Contributions to the public account benefit everyone, including you. What you keep in your private account benefits only you. Your total earnings for each round equal to private tokens kept + public tokens earned.
-At the end of each round, you will see:
-- The total tokens contributed to the public account by all {{participant_label}}s.
-- Your earnings from the public account.
-- Your private tokens kept from the round.
-- Your total earnings so far.
-Answer any question that is posed to you in as much detail as possible and in the format required. Please provide a consistent and coherent response using all the demographic information provided about you. It is crucial for you to accurately replicate the response of a human subject that has the demographic profile you are provided. The human subject response will vary depending on their demographic profile. If you are unsure of an answer, provide a plausible response that is based on all of the information available to you. Do not include your name in your response.</t>
-  </si>
-  <si>
-    <t>Please answer the following questions to ensure you understand the rules. If you contribute 5 tokens to the public account, how many total tokens will be in the public account before it is shared? {response_options}</t>
-  </si>
-  <si>
-    <t>Please answer the following questions to ensure you understand the rules. How are tokens from the public account distributed to group members? {response_options}</t>
-  </si>
-  <si>
-    <t>Please answer the following questions to ensure you understand the rules. If you keep all your tokens in your private account, what happens to the tokens in the public account? {response_options}</t>
-  </si>
-  <si>
-    <t>{"Participant 1": "How many tokens do you want to contribute to the public account? Enter a number between 0 and 10", "Participant 2": "How many tokens do you want to contribute to the public account? Enter a number between 0 and 10", "Participant 3": "How many tokens do you want to contribute to the public account? Enter a number between 0 and 10", "Participant 4": "How many tokens do you want to contribute to the public account? Enter a number between 0 and 10", "Summarizer": "Calculate the following information for each participant in the following format:\n- The total tokens contributed to the public account by all participants:\n- The participant's earnings from the public account:\n- The participant's private tokens kept from the round:\n- The participant's total earnings so far:"}</t>
-  </si>
-  <si>
-    <t>public_good_experiment_sample</t>
   </si>
 </sst>
 </file>
@@ -766,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1002"/>
+  <dimension ref="A1:B1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -792,7 +810,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -811,1072 +829,1080 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
-        <v>4</v>
+        <v>112</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>108</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>10</v>
+      <c r="A12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B14" s="3">
+        <v>104</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="3">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="137" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="164" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="168" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="171" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="174" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="175" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="176" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="177" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="178" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="179" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="180" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="181" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="182" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="184" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="186" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="189" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="191" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="192" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="193" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="194" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="195" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="196" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="197" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="198" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="199" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="200" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="201" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="202" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="203" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="222" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="432" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="433" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="434" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="442" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="443" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="445" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="446" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="450" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="500" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="501" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="502" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="503" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="504" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="505" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="506" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="507" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="508" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="509" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="510" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="511" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="512" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="513" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="514" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="515" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="516" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="517" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="518" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="519" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="520" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="521" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="522" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="523" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="524" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="525" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="526" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="527" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="528" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="529" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="530" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="531" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="532" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="533" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="534" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="535" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="536" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="537" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="538" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="539" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="540" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="541" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="542" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="543" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="544" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="545" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="546" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="547" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="548" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="549" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="550" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="551" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="552" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="553" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="554" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="555" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="556" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="557" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="558" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="559" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="560" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="561" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="562" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="563" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="564" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="565" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="566" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="567" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="568" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="569" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="570" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="571" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="572" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="573" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="574" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="575" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="576" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="577" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="578" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="579" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="580" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="581" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="582" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="583" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="584" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="585" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="586" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="587" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="588" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="589" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="590" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="591" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="592" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="593" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="594" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="595" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="596" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="597" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="598" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="599" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="600" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="601" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="602" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="603" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="604" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="605" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="606" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="607" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="608" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="609" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="610" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="611" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="612" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="613" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="614" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="615" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="616" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="617" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="618" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="619" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="620" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="621" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="622" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="623" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="624" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="625" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="626" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="627" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="628" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="629" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="630" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="631" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="632" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="633" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="634" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="635" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="636" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="637" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="638" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="639" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="640" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="641" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="642" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="643" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="644" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="645" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="646" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="647" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="648" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="649" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="650" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="651" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="652" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="653" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="654" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="655" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="656" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="657" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="658" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="659" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="660" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="661" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="662" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="663" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="664" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="665" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="666" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="667" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="668" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="669" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="670" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="671" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="672" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="673" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="674" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="675" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="676" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="677" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="678" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="679" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="680" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="681" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="682" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="683" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="684" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="685" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="686" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="687" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="688" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="689" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="690" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="691" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="692" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="693" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="694" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="695" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="696" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="697" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="698" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="699" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="700" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="701" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="702" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="703" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="704" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="705" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="706" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="707" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="708" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="709" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="710" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="711" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="712" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="713" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="714" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="715" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="716" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="717" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="718" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="719" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="720" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="721" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="722" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="723" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="724" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="725" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="726" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="727" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="728" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="729" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="730" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="731" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="732" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="733" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="734" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="735" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="736" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="737" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="738" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="739" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="740" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="741" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="742" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="743" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="744" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="745" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="746" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="747" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="748" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="749" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="750" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="751" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="752" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="753" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="754" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="755" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="756" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="757" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="758" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="759" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="760" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="761" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="762" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="763" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="764" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="765" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="766" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="767" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="768" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="769" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="770" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="771" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="772" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="773" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="774" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="775" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="776" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="777" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="778" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="779" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="780" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="781" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="782" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="783" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="784" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="785" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="786" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="787" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="788" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="789" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="790" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="791" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="792" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="793" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="794" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="795" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="796" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="797" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="798" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="799" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="800" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="801" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="802" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="803" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="804" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="805" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="806" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="807" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="808" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="809" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="810" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="811" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="812" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="813" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="814" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="815" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="816" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="817" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="818" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="819" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="820" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="821" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="822" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="823" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="824" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="825" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="826" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="827" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="828" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="829" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="830" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="831" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="832" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="833" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="834" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="835" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="836" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="837" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="838" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="839" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="840" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="841" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="842" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="843" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="844" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="845" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="846" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="847" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="848" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="849" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="850" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="851" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="852" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="853" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="854" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="855" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="856" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="857" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="858" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="859" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="860" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="861" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="862" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="863" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="864" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="865" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="866" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="867" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="868" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="869" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="870" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="871" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="872" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="873" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="874" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="875" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="876" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="877" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="878" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="879" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="880" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="881" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="882" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="883" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="884" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="885" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="886" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="887" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="888" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="889" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="890" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="891" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="892" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="893" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="894" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="895" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="896" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="897" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="898" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="899" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="900" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="901" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="902" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="903" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="904" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="905" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="906" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="907" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="908" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="909" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="910" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="911" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="912" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="913" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="914" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="915" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="916" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="917" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="918" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="919" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="920" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="921" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="922" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="923" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="924" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="925" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="926" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="927" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="928" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="929" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="930" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="931" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="932" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="933" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="934" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="935" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="936" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="937" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="938" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="939" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="940" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="941" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="942" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="943" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="944" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="945" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="946" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="947" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="948" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="949" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="950" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="951" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="952" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="953" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="954" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="955" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="956" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="957" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="958" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="959" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="960" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="961" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="962" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="963" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="964" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="965" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="966" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="967" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="968" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="969" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="970" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="971" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="972" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="973" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="974" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="975" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="976" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="977" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="983" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="984" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="992" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="994" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1001" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1002" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -1887,7 +1913,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2930,7 +2958,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2959,10 +2989,10 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2970,7 +3000,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2978,7 +3008,7 @@
         <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2986,7 +3016,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2994,7 +3024,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3998,16 +4028,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L858"/>
+  <dimension ref="A1:M858"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="33.83203125" style="3" customWidth="1"/>
@@ -4017,11 +4047,12 @@
     <col min="9" max="9" width="39.83203125" style="3" customWidth="1"/>
     <col min="10" max="10" width="25.83203125" style="3" customWidth="1"/>
     <col min="11" max="11" width="18.83203125" style="3" customWidth="1"/>
-    <col min="12" max="28" width="10.6640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" style="3" customWidth="1"/>
+    <col min="13" max="28" width="10.6640625" style="3" customWidth="1"/>
     <col min="29" max="16384" width="11.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>30</v>
       </c>
@@ -4058,8 +4089,11 @@
       <c r="L1" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>113</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -4072,14 +4106,14 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -4092,13 +4126,16 @@
       <c r="L2" s="3">
         <v>0</v>
       </c>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -4107,20 +4144,20 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="J3" s="3">
         <v>1</v>
       </c>
@@ -4130,13 +4167,16 @@
       <c r="L3" s="3">
         <v>1</v>
       </c>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
@@ -4145,20 +4185,20 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="J4" s="3">
         <v>1</v>
       </c>
@@ -4168,13 +4208,16 @@
       <c r="L4" s="3">
         <v>1</v>
       </c>
+      <c r="M4" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="C5" s="2">
         <v>3</v>
@@ -4183,20 +4226,20 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="J5" s="3">
         <v>1</v>
       </c>
@@ -4206,13 +4249,16 @@
       <c r="L5" s="3">
         <v>1</v>
       </c>
+      <c r="M5" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
@@ -4221,19 +4267,19 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="I6" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J6" s="3">
         <v>0</v>
@@ -4244,13 +4290,16 @@
       <c r="L6" s="3">
         <v>0</v>
       </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
       <c r="C7" s="2">
         <v>4</v>
@@ -4259,19 +4308,19 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="I7" s="5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="J7" s="3">
         <v>0</v>
@@ -4282,13 +4331,16 @@
       <c r="L7" s="3">
         <v>0</v>
       </c>
+      <c r="M7" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
       <c r="C8" s="2">
         <v>4</v>
@@ -4297,19 +4349,19 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="I8" s="5" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="J8" s="3">
         <v>0</v>
@@ -4320,13 +4372,16 @@
       <c r="L8" s="3">
         <v>0</v>
       </c>
+      <c r="M8" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
       <c r="C9" s="2">
         <v>4</v>
@@ -4335,19 +4390,19 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="I9" s="5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="J9" s="3">
         <v>0</v>
@@ -4358,13 +4413,16 @@
       <c r="L9" s="3">
         <v>0</v>
       </c>
+      <c r="M9" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
       <c r="C10" s="2">
         <v>4</v>
@@ -4373,19 +4431,19 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="I10" s="5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="J10" s="3">
         <v>0</v>
@@ -4396,13 +4454,16 @@
       <c r="L10" s="3">
         <v>0</v>
       </c>
+      <c r="M10" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5255,8 +5316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AQ515"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5268,64 +5329,64 @@
   <sheetData>
     <row r="1" spans="1:43" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="U1" s="7" t="s">
         <v>11</v>
@@ -5359,64 +5420,64 @@
     </row>
     <row r="2" spans="1:43" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="T2" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="U2" s="7" t="s">
         <v>11</v>
@@ -6529,7 +6590,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6542,7 +6603,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -6550,10 +6611,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed JSON parsing error when using hugging face models.
</commit_message>
<xml_diff>
--- a/demos/public_good_experiment_prompt_template_sample.xlsx
+++ b/demos/public_good_experiment_prompt_template_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondlow/Documents/talking-to-machines/talking-to-machines/demos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008903A3-520D-644A-BDE8-41CC4530EBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF2CB96-654A-BA4A-903F-D40F75D63393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8680" yWindow="760" windowWidth="25880" windowHeight="20240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="-22820" windowWidth="31260" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="experimental_setting" sheetId="1" r:id="rId1"/>
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1003"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4030,7 +4030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M858"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>

</xml_diff>